<commit_message>
manga v(2.10.0.1) Reorgnize the project files
- try to add capability of supporting *.ods files (not tested yet).
- Edit .ignore file
- edit building /exe so that all executable will be there.
- re-write the code of Laounch4J and version part
- fix the bug of ReadingResourceAsStream.
</commit_message>
<xml_diff>
--- a/eqServer/src/test/resources/example.xlsx
+++ b/eqServer/src/test/resources/example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,7 +968,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,7 +1250,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:L1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C9">
       <formula1>"Multiple Choice,Blank Field"</formula1>
     </dataValidation>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>